<commit_message>
ExcelMachineEditor Worksheet 변경시 import() 실행
</commit_message>
<xml_diff>
--- a/Assets/QuickSheet/Example/Excel/ExcelTable.xlsx
+++ b/Assets/QuickSheet/Example/Excel/ExcelTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Unity-QuickSheet\Assets\QuickSheet\Example\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA920662-120E-44C4-AB13-07D025231433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081E7429-CA88-496F-B38D-D1C434DB1FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -123,7 +123,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Type</t>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -131,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,36 +149,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -183,68 +166,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -262,7 +189,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{62F83728-3FDC-43F3-9FE4-1DA3F690B02B}" name="Difficulty" displayName="Difficulty" ref="B3:C6" totalsRowShown="0">
+  <autoFilter ref="B3:C6" xr:uid="{62F83728-3FDC-43F3-9FE4-1DA3F690B02B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5CC18A0D-856C-4BDB-BF39-9AD204D65325}" name="Difficulty"/>
+    <tableColumn id="2" xr3:uid="{BD715D02-0C3C-47FA-94A5-077085E4245B}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A5FBB37-733F-410F-B884-F70D6C503621}" name="Fighter" displayName="Fighter" ref="B2:F12" totalsRowShown="0">
   <autoFilter ref="B2:F12" xr:uid="{1A5FBB37-733F-410F-B884-F70D6C503621}"/>
   <tableColumns count="5">
@@ -276,7 +218,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2572F4E8-6C5D-4E51-8329-24CD5A8CCC1D}" name="Currency" displayName="Currency" ref="B16:C18" totalsRowShown="0">
   <autoFilter ref="B16:C18" xr:uid="{2572F4E8-6C5D-4E51-8329-24CD5A8CCC1D}"/>
   <tableColumns count="2">
@@ -584,52 +526,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61738ADB-AB45-4F77-9C11-1586893678BB}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.625" customWidth="1"/>
+    <col min="2" max="2" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -638,7 +584,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -695,7 +641,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -746,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -797,7 +743,7 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -869,17 +815,5 @@
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBB6CECC-8B1A-484A-BB3A-6E15DE29AEF4}">
-          <x14:formula1>
-            <xm:f>Enums!$B$3:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature - Enum Generate
</commit_message>
<xml_diff>
--- a/Assets/QuickSheet/Example/Excel/ExcelTable.xlsx
+++ b/Assets/QuickSheet/Example/Excel/ExcelTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Unity-QuickSheet\Assets\QuickSheet\Example\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geekchic\Documents\Unity Projects\Unity-QuickSheet\Assets\QuickSheet\Example\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081E7429-CA88-496F-B38D-D1C434DB1FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754C946B-4A3C-4488-B8B4-A601C2A09675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1230" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enums" sheetId="2" r:id="rId1"/>
@@ -119,14 +119,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
-    <t>Difficulty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -189,16 +189,12 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{62F83728-3FDC-43F3-9FE4-1DA3F690B02B}" name="Difficulty" displayName="Difficulty" ref="B3:C6" totalsRowShown="0">
   <autoFilter ref="B3:C6" xr:uid="{62F83728-3FDC-43F3-9FE4-1DA3F690B02B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5CC18A0D-856C-4BDB-BF39-9AD204D65325}" name="Difficulty"/>
-    <tableColumn id="2" xr3:uid="{BD715D02-0C3C-47FA-94A5-077085E4245B}" name="Value"/>
+    <tableColumn id="2" xr3:uid="{0189F6DF-8E72-4B15-B314-99CF0CC75FBA}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -529,7 +525,7 @@
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -539,10 +535,10 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -584,7 +580,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -641,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>

</xml_diff>